<commit_message>
edit SkillSystem _ Icon
Player에 저장된 SkillData를 기반으로 스킬 아이콘 변경
</commit_message>
<xml_diff>
--- a/GameDesign/데이터 테이블/SkillTable.xlsx
+++ b/GameDesign/데이터 테이블/SkillTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca2aeba951d90199/문서/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\portfolio\Unity\Unity_Study\Team_Pearl\Team_Pearl\GameDesign\데이터 테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7B837C4-FE85-4FF0-A2A4-75D58A1EC3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889E9878-6225-4F8E-B875-D5587D73B231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="2055" windowWidth="16230" windowHeight="11385" xr2:uid="{340D970B-A38D-4908-AE97-4360A0CB6FCD}"/>
+    <workbookView xWindow="38400" yWindow="5445" windowWidth="21600" windowHeight="18900" xr2:uid="{340D970B-A38D-4908-AE97-4360A0CB6FCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -551,21 +551,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFD71C0-49BA-4ECB-97DA-3902CEC3BF58}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.875" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="17.25" customWidth="1"/>
+    <col min="6" max="6" width="22.75" customWidth="1"/>
+    <col min="7" max="7" width="11.75" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
     <col min="9" max="9" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -622,8 +627,11 @@
       <c r="I2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -651,8 +659,11 @@
       <c r="I3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -680,8 +691,11 @@
       <c r="I4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -709,8 +723,11 @@
       <c r="I5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -738,8 +755,11 @@
       <c r="I6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -767,8 +787,11 @@
       <c r="I7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -796,8 +819,11 @@
       <c r="I8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -825,8 +851,11 @@
       <c r="I9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -854,8 +883,11 @@
       <c r="I10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -883,8 +915,11 @@
       <c r="I11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -912,8 +947,11 @@
       <c r="I12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -941,8 +979,11 @@
       <c r="I13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -970,8 +1011,11 @@
       <c r="I14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -999,8 +1043,11 @@
       <c r="I15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1027,6 +1074,9 @@
       </c>
       <c r="I16" t="s">
         <v>36</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>